<commit_message>
downloaded RT News, and APK Extractors. Downloaded Dex2Jar and applied it the apks. Unzipped the jars.  RT News has much more too look at the APK Extractor, so it seems.
</commit_message>
<xml_diff>
--- a/AndroidPermissionsWorksheet.xlsx
+++ b/AndroidPermissionsWorksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreasslovacek/Android_Research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA85A7FD-A1C9-BE4B-91F3-75F1095349B7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD38278-4018-E04A-9AB9-746A45D608F3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" xr2:uid="{44804EE6-5D3F-B748-AABC-471406EE43A8}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Manifest.Permissions!$A$1:$G$152</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1404,11 +1404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA885B7-9509-5E49-8D1C-9BA3B00F1941}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:G152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D154" sqref="D154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1454,7 +1453,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
@@ -1533,7 +1532,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
@@ -1564,7 +1563,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
@@ -1581,7 +1580,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
@@ -1640,7 +1639,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
@@ -1671,7 +1670,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
@@ -1688,7 +1687,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -1719,7 +1718,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
@@ -1750,7 +1749,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
@@ -1781,7 +1780,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
@@ -1792,7 +1791,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>26</v>
       </c>
@@ -1803,7 +1802,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
@@ -1814,7 +1813,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
@@ -1825,7 +1824,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
@@ -1836,7 +1835,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>26</v>
       </c>
@@ -1847,7 +1846,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
@@ -1858,7 +1857,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>26</v>
       </c>
@@ -1869,7 +1868,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>26</v>
       </c>
@@ -1880,7 +1879,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
@@ -1891,7 +1890,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>26</v>
       </c>
@@ -1902,7 +1901,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>26</v>
       </c>
@@ -1913,7 +1912,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>26</v>
       </c>
@@ -1952,7 +1951,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>26</v>
       </c>
@@ -1969,7 +1968,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>26</v>
       </c>
@@ -1980,7 +1979,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>26</v>
       </c>
@@ -1991,7 +1990,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>26</v>
       </c>
@@ -2002,7 +2001,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>26</v>
       </c>
@@ -2013,7 +2012,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>26</v>
       </c>
@@ -2024,7 +2023,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>26</v>
       </c>
@@ -2035,7 +2034,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>26</v>
       </c>
@@ -2046,7 +2045,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>26</v>
       </c>
@@ -2057,7 +2056,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>26</v>
       </c>
@@ -2068,7 +2067,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>26</v>
       </c>
@@ -2079,7 +2078,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>26</v>
       </c>
@@ -2090,7 +2089,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>26</v>
       </c>
@@ -2101,7 +2100,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>26</v>
       </c>
@@ -2112,7 +2111,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>26</v>
       </c>
@@ -2123,7 +2122,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>26</v>
       </c>
@@ -2134,7 +2133,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>26</v>
       </c>
@@ -2145,7 +2144,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>26</v>
       </c>
@@ -2156,7 +2155,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>26</v>
       </c>
@@ -2167,7 +2166,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>26</v>
       </c>
@@ -2178,7 +2177,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>26</v>
       </c>
@@ -2189,7 +2188,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>26</v>
       </c>
@@ -2200,7 +2199,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>26</v>
       </c>
@@ -2211,7 +2210,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>26</v>
       </c>
@@ -2222,7 +2221,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>26</v>
       </c>
@@ -2233,7 +2232,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="64" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>26</v>
       </c>
@@ -2244,7 +2243,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>26</v>
       </c>
@@ -2255,7 +2254,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="66" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>26</v>
       </c>
@@ -2266,7 +2265,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>26</v>
       </c>
@@ -2277,7 +2276,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>26</v>
       </c>
@@ -2288,7 +2287,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>26</v>
       </c>
@@ -2299,7 +2298,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>26</v>
       </c>
@@ -2310,7 +2309,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="71" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>26</v>
       </c>
@@ -2321,7 +2320,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>26</v>
       </c>
@@ -2332,7 +2331,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>26</v>
       </c>
@@ -2343,7 +2342,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>26</v>
       </c>
@@ -2354,7 +2353,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>26</v>
       </c>
@@ -2365,7 +2364,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>26</v>
       </c>
@@ -2376,7 +2375,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="77" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>26</v>
       </c>
@@ -2387,7 +2386,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>26</v>
       </c>
@@ -2398,7 +2397,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>26</v>
       </c>
@@ -2409,7 +2408,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="80" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>26</v>
       </c>
@@ -2420,7 +2419,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>26</v>
       </c>
@@ -2431,7 +2430,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="82" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>26</v>
       </c>
@@ -2442,7 +2441,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="83" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>26</v>
       </c>
@@ -2453,7 +2452,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="84" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>26</v>
       </c>
@@ -2464,7 +2463,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="85" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>26</v>
       </c>
@@ -2475,7 +2474,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="86" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>26</v>
       </c>
@@ -2486,7 +2485,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="87" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>26</v>
       </c>
@@ -2497,7 +2496,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="88" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>26</v>
       </c>
@@ -2508,7 +2507,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="89" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>26</v>
       </c>
@@ -2519,7 +2518,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="90" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>26</v>
       </c>
@@ -2530,7 +2529,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="91" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>26</v>
       </c>
@@ -2541,7 +2540,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="92" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>26</v>
       </c>
@@ -2552,7 +2551,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="93" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>26</v>
       </c>
@@ -2563,7 +2562,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="94" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>26</v>
       </c>
@@ -2574,7 +2573,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="95" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>26</v>
       </c>
@@ -2585,7 +2584,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="96" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>26</v>
       </c>
@@ -2596,7 +2595,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>26</v>
       </c>
@@ -2607,7 +2606,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>26</v>
       </c>
@@ -2618,7 +2617,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>26</v>
       </c>
@@ -2629,7 +2628,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>26</v>
       </c>
@@ -2640,7 +2639,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>26</v>
       </c>
@@ -2651,7 +2650,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>26</v>
       </c>
@@ -2662,7 +2661,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="103" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>26</v>
       </c>
@@ -2673,7 +2672,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>26</v>
       </c>
@@ -2684,7 +2683,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>26</v>
       </c>
@@ -2695,7 +2694,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>26</v>
       </c>
@@ -2706,7 +2705,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>26</v>
       </c>
@@ -2717,7 +2716,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>26</v>
       </c>
@@ -2728,7 +2727,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>26</v>
       </c>
@@ -2739,7 +2738,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>26</v>
       </c>
@@ -2750,7 +2749,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>26</v>
       </c>
@@ -2761,7 +2760,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>26</v>
       </c>
@@ -2772,7 +2771,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="113" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>26</v>
       </c>
@@ -2783,7 +2782,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="114" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>26</v>
       </c>
@@ -2794,7 +2793,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="115" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>26</v>
       </c>
@@ -2805,7 +2804,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="116" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>26</v>
       </c>
@@ -2816,7 +2815,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="117" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>26</v>
       </c>
@@ -2827,7 +2826,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="118" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>26</v>
       </c>
@@ -2838,7 +2837,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="119" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>26</v>
       </c>
@@ -2849,7 +2848,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="120" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>26</v>
       </c>
@@ -2860,7 +2859,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="121" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>26</v>
       </c>
@@ -2871,7 +2870,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="122" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>26</v>
       </c>
@@ -2882,7 +2881,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="123" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>26</v>
       </c>
@@ -2893,7 +2892,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="124" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>26</v>
       </c>
@@ -2904,7 +2903,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="125" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>26</v>
       </c>
@@ -2915,7 +2914,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="126" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>26</v>
       </c>
@@ -2926,7 +2925,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="127" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>26</v>
       </c>
@@ -2937,7 +2936,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="128" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>26</v>
       </c>
@@ -2948,7 +2947,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="129" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>26</v>
       </c>
@@ -2959,7 +2958,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="130" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>26</v>
       </c>
@@ -2970,7 +2969,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="131" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>26</v>
       </c>
@@ -2981,7 +2980,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="132" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>26</v>
       </c>
@@ -2992,7 +2991,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="133" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>26</v>
       </c>
@@ -3003,7 +3002,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="134" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>26</v>
       </c>
@@ -3014,7 +3013,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="135" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>26</v>
       </c>
@@ -3025,7 +3024,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="136" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>26</v>
       </c>
@@ -3036,7 +3035,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="137" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>26</v>
       </c>
@@ -3047,7 +3046,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="138" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>26</v>
       </c>
@@ -3058,7 +3057,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="139" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>26</v>
       </c>
@@ -3069,7 +3068,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="140" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>26</v>
       </c>
@@ -3080,7 +3079,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="141" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>26</v>
       </c>
@@ -3091,7 +3090,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="142" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>26</v>
       </c>
@@ -3102,7 +3101,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="143" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>26</v>
       </c>
@@ -3113,7 +3112,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="144" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>26</v>
       </c>
@@ -3124,7 +3123,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="145" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>26</v>
       </c>
@@ -3135,7 +3134,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="146" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
         <v>26</v>
       </c>
@@ -3146,7 +3145,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="147" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>26</v>
       </c>
@@ -3157,7 +3156,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="148" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>26</v>
       </c>
@@ -3168,7 +3167,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="149" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>26</v>
       </c>
@@ -3179,7 +3178,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="150" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
         <v>26</v>
       </c>
@@ -3190,7 +3189,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="151" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>26</v>
       </c>
@@ -3201,7 +3200,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="152" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>26</v>
       </c>
@@ -3213,45 +3212,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" ref="A1:G152" xr:uid="{B2E33894-9F30-2846-A4A9-6BB7CCC5AD78}">
-    <filterColumn colId="3">
-      <filters>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <x14:filter val="Access network provider at location, or approximate provider without getting location fix; add NMEA listener and more https://developer.android.com/reference/android/location/LocationManager#sendExtraCommand%28java.lang.String,%20java.lang.String,%20android.os.Bundle%29"/>
-            <x14:filter val="Allows access to usernames and passwords"/>
-            <x14:filter val="Allows an app to access approximate location."/>
-            <x14:filter val="Collect network stats from users"/>
-            <x14:filter val="Collect wifi login information"/>
-            <x14:filter val="Could extend VPN solutions to monitor traffic"/>
-            <x14:filter val="If an app wants to provide a UI during calls this is required. https://developer.android.com/reference/android/telecom/InCallService"/>
-            <x14:filter val="If the app is security aware then this is required. https://developer.android.com/guide/topics/admin/device-admin"/>
-            <x14:filter val="Necessary if VR devices will be monitored"/>
-            <x14:filter val="Required for apps that assist disabled users"/>
-            <x14:filter val="Required when the user is asked to choose what app to complete an action with"/>
-            <x14:filter val="Researchers may want to know how a phones batter is performing"/>
-            <x14:filter val="Track user location"/>
-            <x14:filter val="Transer user to research app so voice and transcripts of calls can be analyzed"/>
-          </mc:Choice>
-          <mc:Fallback>
-            <filter val="Allows access to usernames and passwords"/>
-            <filter val="Allows an app to access approximate location."/>
-            <filter val="Collect network stats from users"/>
-            <filter val="Collect wifi login information"/>
-            <filter val="Could extend VPN solutions to monitor traffic"/>
-            <filter val="If an app wants to provide a UI during calls this is required. https://developer.android.com/reference/android/telecom/InCallService"/>
-            <filter val="If the app is security aware then this is required. https://developer.android.com/guide/topics/admin/device-admin"/>
-            <filter val="Necessary if VR devices will be monitored"/>
-            <filter val="Required for apps that assist disabled users"/>
-            <filter val="Required when the user is asked to choose what app to complete an action with"/>
-            <filter val="Researchers may want to know how a phones batter is performing"/>
-            <filter val="Track user location"/>
-            <filter val="Transer user to research app so voice and transcripts of calls can be analyzed"/>
-          </mc:Fallback>
-        </mc:AlternateContent>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G152" xr:uid="{B2E33894-9F30-2846-A4A9-6BB7CCC5AD78}"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="https://developer.android.com/reference/java/lang/String.html" xr:uid="{A7951809-47F8-8848-87D3-EF3FDE970C9B}"/>
     <hyperlink ref="B2" r:id="rId2" location="ACCEPT_HANDOVER" display="https://developer.android.com/reference/android/Manifest.permission.html - ACCEPT_HANDOVER" xr:uid="{58812EE0-8544-DD4B-91A7-775FA6417578}"/>

</xml_diff>